<commit_message>
Change timeout of shutdown for lora-gateway from 8 to 20 seconds
</commit_message>
<xml_diff>
--- a/Docs/AT-SF1P.CBL07.xlsx
+++ b/Docs/AT-SF1P.CBL07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\SF-1P\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75627DCF-14E3-4D7B-AB56-7197F307FF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43B14E6-9054-4758-9D4F-CA3BBECCCF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5940" yWindow="765" windowWidth="21315" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,10 +119,10 @@
     <t>18-1569-BLK</t>
   </si>
   <si>
-    <t>18-1569-Yellow-Green</t>
-  </si>
-  <si>
-    <t>18-1569-BLK+RED+YG</t>
+    <t>18-1569-YEL/GRN</t>
+  </si>
+  <si>
+    <t>18-1569-BLK+RED+YEL/GRN</t>
   </si>
 </sst>
 </file>
@@ -670,14 +670,14 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>